<commit_message>
add results from latest run
</commit_message>
<xml_diff>
--- a/Nowcasts/2025Q3/tables/nowcasts_2025Q3_Nr10_Np1_Nj0.xlsx
+++ b/Nowcasts/2025Q3/tables/nowcasts_2025Q3_Nr10_Np1_Nj0.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Row</t>
   </si>
@@ -106,6 +106,72 @@
   </si>
   <si>
     <t>2025-08-15</t>
+  </si>
+  <si>
+    <t>Prognose</t>
+  </si>
+  <si>
+    <t>surveys</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>turnover</t>
+  </si>
+  <si>
+    <t>financial</t>
+  </si>
+  <si>
+    <t>labor market</t>
+  </si>
+  <si>
+    <t>prices</t>
+  </si>
+  <si>
+    <t>national accounts</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>2025-03-30</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
+  </si>
+  <si>
+    <t>2025-05-15</t>
+  </si>
+  <si>
+    <t>2025-05-30</t>
+  </si>
+  <si>
+    <t>2025-06-15</t>
+  </si>
+  <si>
+    <t>2025-06-30</t>
+  </si>
+  <si>
+    <t>2025-07-15</t>
+  </si>
+  <si>
+    <t>2025-07-30</t>
+  </si>
+  <si>
+    <t>2025-08-15</t>
+  </si>
+  <si>
+    <t>2025-08-30</t>
   </si>
   <si>
     <t>Prognose</t>
@@ -181,63 +247,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.37890625" customWidth="true"/>
     <col min="2" max="2" width="14.24609375" customWidth="true"/>
-    <col min="3" max="3" width="15.24609375" customWidth="true"/>
+    <col min="3" max="3" width="15.64453125" customWidth="true"/>
     <col min="4" max="4" width="14.64453125" customWidth="true"/>
     <col min="5" max="5" width="15.24609375" customWidth="true"/>
     <col min="6" max="6" width="15.77734375" customWidth="true"/>
     <col min="7" max="7" width="15.24609375" customWidth="true"/>
     <col min="8" max="8" width="16.24609375" customWidth="true"/>
     <col min="9" max="9" width="14.64453125" customWidth="true"/>
-    <col min="10" max="10" width="15.77734375" customWidth="true"/>
+    <col min="10" max="10" width="15.046875" customWidth="true"/>
     <col min="11" max="11" width="15.64453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0">
-        <v>0.24094618552374619</v>
+        <v>0.24080207187219643</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
@@ -269,317 +335,352 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B3" s="0">
-        <v>0.28427819787347169</v>
+        <v>0.28436211342840439</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>0.0013402292145429677</v>
+        <v>0.0012439662374659714</v>
       </c>
       <c r="E3" s="0">
-        <v>-0.0037889994458148893</v>
+        <v>-0.0037817599196970104</v>
       </c>
       <c r="F3" s="0">
-        <v>-0.0026062180858059084</v>
+        <v>-0.0025283334682744876</v>
       </c>
       <c r="G3" s="0">
-        <v>0.015097587311249154</v>
+        <v>0.015146769417247196</v>
       </c>
       <c r="H3" s="0">
-        <v>-0.00057928361492928294</v>
+        <v>-0.00057838198981614408</v>
       </c>
       <c r="I3" s="0">
-        <v>0.033801930358175511</v>
+        <v>0.033991010788495674</v>
       </c>
       <c r="J3" s="0">
         <v>0</v>
       </c>
       <c r="K3" s="0">
-        <v>6.6766612307950224e-05</v>
+        <v>6.6770490786766112e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0">
-        <v>0.28220772266371208</v>
+        <v>0.28208020537492945</v>
       </c>
       <c r="C4" s="0">
-        <v>-0.0032376399355991759</v>
+        <v>-0.0035241831576743455</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>-0.0015689660086845207</v>
+        <v>-0.0015560534800836596</v>
       </c>
       <c r="F4" s="0">
-        <v>-7.7426492564115757e-05</v>
+        <v>-7.8031851677072832e-05</v>
       </c>
       <c r="G4" s="0">
         <v>0</v>
       </c>
       <c r="H4" s="0">
-        <v>-0.0019351271466367035</v>
+        <v>-0.0019327886606760635</v>
       </c>
       <c r="I4" s="0">
-        <v>0.0045128965940593934</v>
+        <v>0.0045734133020846612</v>
       </c>
       <c r="J4" s="0">
-        <v>-1.9639384880579047e-05</v>
+        <v>-1.9697362304567411e-05</v>
       </c>
       <c r="K4" s="0">
-        <v>0.00025542716454607373</v>
+        <v>0.00025543315685611079</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0">
-        <v>0.21118733951251933</v>
+        <v>0.2118210139814253</v>
       </c>
       <c r="C5" s="0">
-        <v>-0.00078730530096737935</v>
+        <v>0.00017098688669906457</v>
       </c>
       <c r="D5" s="0">
-        <v>-0.021327128125990379</v>
+        <v>-0.021669175339521635</v>
       </c>
       <c r="E5" s="0">
-        <v>-0.0059972711830854628</v>
+        <v>-0.0061503162577170624</v>
       </c>
       <c r="F5" s="0">
-        <v>0.0029198895211829355</v>
+        <v>0.0031600996313077712</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.05604137488368012</v>
+        <v>-0.055992514771728279</v>
       </c>
       <c r="H5" s="0">
-        <v>-0.00063200185474940611</v>
+        <v>-0.00062809303110503947</v>
       </c>
       <c r="I5" s="0">
-        <v>0.010731672550850294</v>
+        <v>0.010736702060784356</v>
       </c>
       <c r="J5" s="0">
         <v>0</v>
       </c>
       <c r="K5" s="0">
-        <v>0.00011313612524677108</v>
+        <v>0.00011311942777669781</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0">
-        <v>0.37871817174340416</v>
+        <v>0.37974679247291698</v>
       </c>
       <c r="C6" s="0">
-        <v>0.21334443265068179</v>
+        <v>0.21468273181312142</v>
       </c>
       <c r="D6" s="0">
         <v>0</v>
       </c>
       <c r="E6" s="0">
-        <v>0.0033789270405524068</v>
+        <v>0.0033733487000692638</v>
       </c>
       <c r="F6" s="0">
-        <v>0.00017505046289315734</v>
+        <v>0.00018191970818550758</v>
       </c>
       <c r="G6" s="0">
         <v>0</v>
       </c>
       <c r="H6" s="0">
-        <v>0.00069869584423049242</v>
+        <v>0.00070713972826768798</v>
       </c>
       <c r="I6" s="0">
-        <v>-0.0500848069774288</v>
+        <v>-0.051037856639376288</v>
       </c>
       <c r="J6" s="0">
         <v>0</v>
       </c>
       <c r="K6" s="0">
-        <v>1.8533209955789998e-05</v>
+        <v>1.8495181224098545e-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B7" s="0">
-        <v>0.38591072502269214</v>
+        <v>0.38619987317568699</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>-0.040204025309234906</v>
+        <v>-0.040400119627963769</v>
       </c>
       <c r="E7" s="0">
-        <v>0.012342786954494185</v>
+        <v>0.011964863103795773</v>
       </c>
       <c r="F7" s="0">
-        <v>0.012658677282629711</v>
+        <v>0.012449969319882239</v>
       </c>
       <c r="G7" s="0">
-        <v>0.015593115834815392</v>
+        <v>0.015643289302739314</v>
       </c>
       <c r="H7" s="0">
         <v>0</v>
       </c>
       <c r="I7" s="0">
-        <v>0.0047681254213007892</v>
+        <v>0.0047611922848377463</v>
       </c>
       <c r="J7" s="0">
         <v>0</v>
       </c>
       <c r="K7" s="0">
-        <v>0.002033873095282801</v>
+        <v>0.002033886319478706</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B8" s="0">
-        <v>0.31808962084937442</v>
+        <v>0.31795258949313859</v>
       </c>
       <c r="C8" s="0">
-        <v>0.005113368003438333</v>
+        <v>0.0037618529577373543</v>
       </c>
       <c r="D8" s="0">
         <v>0</v>
       </c>
       <c r="E8" s="0">
-        <v>-0.01545286950442412</v>
+        <v>-0.015389088370375149</v>
       </c>
       <c r="F8" s="0">
-        <v>-0.015405444488849894</v>
+        <v>-0.015394683700806744</v>
       </c>
       <c r="G8" s="0">
         <v>0</v>
       </c>
       <c r="H8" s="0">
-        <v>-3.3402636028691631e-05</v>
+        <v>-3.2896263434469691e-05</v>
       </c>
       <c r="I8" s="0">
-        <v>-0.043927054307796205</v>
+        <v>-0.04307682182660006</v>
       </c>
       <c r="J8" s="0">
         <v>0</v>
       </c>
       <c r="K8" s="0">
-        <v>0.0018842987603428507</v>
+        <v>0.0018843535209306927</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.06885817027519342</v>
+        <v>-0.071497957548829705</v>
       </c>
       <c r="C9" s="0">
         <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>-0.23840030890923083</v>
+        <v>-0.23930056372694083</v>
       </c>
       <c r="E9" s="0">
-        <v>-0.006408437579805853</v>
+        <v>-0.0064611883494527936</v>
       </c>
       <c r="F9" s="0">
-        <v>-0.13825916220252646</v>
+        <v>-0.13977766188943633</v>
       </c>
       <c r="G9" s="0">
-        <v>-0.008705944306807066</v>
+        <v>-0.0087111813587890073</v>
       </c>
       <c r="H9" s="0">
-        <v>-0.0017654183961398613</v>
+        <v>-0.0017849062377760128</v>
       </c>
       <c r="I9" s="0">
-        <v>0.0047746607425412533</v>
+        <v>0.0047681202030623376</v>
       </c>
       <c r="J9" s="0">
         <v>0</v>
       </c>
       <c r="K9" s="0">
-        <v>0.0018168195274009258</v>
+        <v>0.0018168343173642909</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0">
-        <v>0.046433417111353903</v>
+        <v>0.054566760516671781</v>
       </c>
       <c r="C10" s="0">
-        <v>0.16627865679398982</v>
+        <v>0.17759045202830737</v>
       </c>
       <c r="D10" s="0">
         <v>0</v>
       </c>
       <c r="E10" s="0">
-        <v>0.0020475952942650526</v>
+        <v>0.0020123662740876092</v>
       </c>
       <c r="F10" s="0">
-        <v>0.0019351123776234474</v>
+        <v>0.0018983461025653334</v>
       </c>
       <c r="G10" s="0">
         <v>0</v>
       </c>
       <c r="H10" s="0">
-        <v>-0.00053485562364508153</v>
+        <v>-0.00053475956616136713</v>
       </c>
       <c r="I10" s="0">
-        <v>0.040476439553013041</v>
+        <v>0.040294149890125641</v>
       </c>
       <c r="J10" s="0">
-        <v>-0.10460181508185677</v>
+        <v>-0.10488631362318888</v>
       </c>
       <c r="K10" s="0">
-        <v>0.0096904540731578143</v>
+        <v>0.0096904769597657703</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B11" s="0">
-        <v>0.29908633578388283</v>
+        <v>0.30558649411408689</v>
       </c>
       <c r="C11" s="0">
         <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>0.41217356707150815</v>
+        <v>0.41040944622830727</v>
       </c>
       <c r="E11" s="0">
-        <v>-0.082151305157122878</v>
+        <v>-0.08157479969732763</v>
       </c>
       <c r="F11" s="0">
-        <v>-0.17672202658548417</v>
+        <v>-0.17758697045414956</v>
       </c>
       <c r="G11" s="0">
-        <v>-0.033460783624977716</v>
+        <v>-0.033618800681720573</v>
       </c>
       <c r="H11" s="0">
-        <v>-0.00078300217652895647</v>
+        <v>-0.00078157726851500135</v>
       </c>
       <c r="I11" s="0">
-        <v>0.10125963445734582</v>
+        <v>0.10183556307617514</v>
       </c>
       <c r="J11" s="0">
         <v>0</v>
       </c>
       <c r="K11" s="0">
-        <v>0.032336834687788668</v>
+        <v>0.032336872394645472</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0.086829374710636814</v>
+      </c>
+      <c r="C12" s="0">
+        <v>-0.12507595826134951</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0">
+        <v>-0.0019631484652427259</v>
+      </c>
+      <c r="F12" s="0">
+        <v>-0.0018500681955330132</v>
+      </c>
+      <c r="G12" s="0">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0">
+        <v>-0.00024982997216308985</v>
+      </c>
+      <c r="I12" s="0">
+        <v>-0.042613970191810242</v>
+      </c>
+      <c r="J12" s="0">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0">
+        <v>-0.047004144317351504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>